<commit_message>
carga del excel lista
</commit_message>
<xml_diff>
--- a/personaContacto/subidas/3_AFILIADOS_personas.xlsx
+++ b/personaContacto/subidas/3_AFILIADOS_personas.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IHC-LCCSF\personaContacto\subidas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Cedula</t>
   </si>
@@ -41,97 +37,102 @@
     <t>Telefono</t>
   </si>
   <si>
+    <t>V21443181</t>
+  </si>
+  <si>
+    <t>Argenis</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
+    <t>4127849712 454548</t>
+  </si>
+  <si>
+    <t>V20699411</t>
+  </si>
+  <si>
+    <t>Ivonne</t>
+  </si>
+  <si>
+    <t>Ortega</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
-    <t>V21443181</t>
-  </si>
-  <si>
-    <t>4127849712 454548</t>
-  </si>
-  <si>
-    <t>Argenis</t>
-  </si>
-  <si>
-    <t>García</t>
-  </si>
-  <si>
-    <t>V5890112</t>
-  </si>
-  <si>
-    <t>Eleazar</t>
-  </si>
-  <si>
-    <t>Fajardo</t>
-  </si>
-  <si>
-    <t>V12187990</t>
-  </si>
-  <si>
-    <t>Camila</t>
-  </si>
-  <si>
-    <t>Rojas</t>
+    <t>V123456789</t>
+  </si>
+  <si>
+    <t>Priscilla</t>
+  </si>
+  <si>
+    <t>BlaBla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
+      <strike val="0"/>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="14" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -173,13 +174,13 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Jpan" typeface="?? ?????"/>
+        <a:font script="Hang" typeface="?? ??"/>
+        <a:font script="Hans" typeface="??"/>
+        <a:font script="Hant" typeface="????"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -205,16 +206,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Jpan" typeface="?? ?????"/>
+        <a:font script="Hang" typeface="?? ??"/>
+        <a:font script="Hans" typeface="??"/>
+        <a:font script="Hant" typeface="????"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -240,7 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -416,16 +415,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,47 +445,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>34061</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1">
+        <v>34270</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1">
-        <v>19865</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
       <c r="F3">
-        <v>4168807788</v>
+        <v>123456</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -496,40 +496,79 @@
         <v>17</v>
       </c>
       <c r="D4" s="1">
-        <v>31820</v>
+        <v>32916</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F4">
-        <v>4126679987</v>
+        <v>23435234</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>